<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => dioxins
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/dioxine_like/summarised_levels_data_dioxine_like_TEQ.xlsx
+++ b/inst/results/data_contam/dioxine_like/summarised_levels_data_dioxine_like_TEQ.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,12 +375,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>median_1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median_2</t>
+          <t>median_percent</t>
         </is>
       </c>
     </row>
@@ -396,13 +391,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.0029061</v>
+        <v>0.00106495</v>
       </c>
       <c r="D2">
-        <v>2.031</v>
-      </c>
-      <c r="E2">
-        <v>44.71</v>
+        <v>16.38384615384615</v>
       </c>
     </row>
     <row r="3">
@@ -417,13 +409,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.00331005</v>
+        <v>0.0030336</v>
       </c>
       <c r="D3">
-        <v>7.985</v>
-      </c>
-      <c r="E3">
-        <v>50.92</v>
+        <v>46.67076923076923</v>
       </c>
     </row>
     <row r="4">
@@ -438,13 +427,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.01648435</v>
+        <v>0.017437</v>
       </c>
       <c r="D4">
-        <v>71.55</v>
-      </c>
-      <c r="E4">
-        <v>253.6</v>
+        <v>268.2615384615385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>